<commit_message>
add user-role for process order
</commit_message>
<xml_diff>
--- a/doc/组织过程资产/SA权限.xlsx
+++ b/doc/组织过程资产/SA权限.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>依勤 SA 权限</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -41,131 +41,151 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>订单管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>超级管理员管理</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>管理员管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>客户管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户管理 - 客户管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户折扣</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>属性管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品管理 - 属性管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除所有属性</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>追加属性</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除属性</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>编辑属性</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品内容管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品管理 - 商品内容管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除所有商品</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>追加商品</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除商品</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>编辑商品</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>快速购物管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户管理 - 管理员管理（超管管理页面）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户管理 - 管理员管理（管理员自身管理页面）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>品牌管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品管理 - 品牌管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>追加品牌</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除品牌</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>编辑品牌</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单删除</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单修改</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>用户管理 - 超级管理员管理</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>管理员管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>客户管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户管理 - 客户管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户折扣</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>属性管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品管理 - 属性管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>删除所有属性</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>追加属性</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>删除属性</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>编辑属性</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品内容管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品管理 - 商品内容管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>删除所有商品</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>追加商品</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>删除商品</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>编辑商品</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>快速购物管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>管理员管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户管理 - 管理员管理（超管管理页面）</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户管理 - 管理员管理（管理员自身管理页面）</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>品牌管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品管理 - 品牌管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>追加品牌</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>删除品牌</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>编辑品牌</t>
+    <t>订单管理 - 订单删除</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单管理 - 订单修改</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单管理 - 订单状态修改</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单状态修改</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -596,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -634,249 +654,282 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3">
-        <v>12000</v>
+        <v>11001</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3">
-        <v>12100</v>
+        <v>11002</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3">
-        <v>12200</v>
+        <v>11003</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3">
-        <v>12300</v>
+        <v>12000</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3">
-        <v>12301</v>
+        <v>12100</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="3">
-        <v>12400</v>
+        <v>12200</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="3">
-        <v>13000</v>
+        <v>12300</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="3">
-        <v>13100</v>
+        <v>12301</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="3">
-        <v>13101</v>
+        <v>12400</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="3">
-        <v>13102</v>
+        <v>13000</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="3">
-        <v>13103</v>
+        <v>13100</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3">
-        <v>13104</v>
+        <v>13101</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3">
-        <v>13200</v>
+        <v>13102</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3">
-        <v>13201</v>
+        <v>13103</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="3">
-        <v>13202</v>
+        <v>13104</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3">
-        <v>13203</v>
+        <v>13200</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="3">
-        <v>13204</v>
+        <v>13201</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="3">
-        <v>13300</v>
+        <v>13202</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3">
-        <v>13302</v>
+        <v>13203</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="3">
-        <v>13303</v>
+        <v>13204</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="3">
-        <v>13304</v>
+        <v>13300</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="3">
+        <v>13302</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="3">
+        <v>13303</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="3">
+        <v>13304</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="3">
         <v>14000</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>28</v>
+      <c r="B29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add product index list
</commit_message>
<xml_diff>
--- a/doc/组织过程资产/SA权限.xlsx
+++ b/doc/组织过程资产/SA权限.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>依勤 SA 权限</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -213,19 +213,27 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>商品管理 - 特色商品管理（首页商品列表）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>特色商品管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>邀请码管理</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>邀请码管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>特色商品管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品管理 - 特色商品管理（首页商品列表）</t>
+    <t>系统设定管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统设定管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统设定管理 － 邀请码管理</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -313,8 +321,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -380,7 +400,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="21">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -389,6 +409,8 @@
     <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -397,6 +419,8 @@
     <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -696,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -1083,41 +1107,52 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3">
-        <v>13500</v>
+        <v>14000</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="1">
-        <v>160730</v>
-      </c>
-      <c r="E34" s="1">
-        <v>3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3">
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3">
-        <v>15000</v>
+        <v>15100</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="3">
+        <v>15200</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>49</v>
+      <c r="D37" s="1">
+        <v>160730</v>
+      </c>
+      <c r="E37" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add role for upload-image
</commit_message>
<xml_diff>
--- a/doc/组织过程资产/SA权限.xlsx
+++ b/doc/组织过程资产/SA权限.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taosijun/git/yiqin/doc/组织过程资产/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="SA权限" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
   <si>
     <t>依勤 SA 权限</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -238,6 +246,37 @@
   </si>
   <si>
     <t>导出商品</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>图片管理</t>
+    <rPh sb="0" eb="1">
+      <t>tu p</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>guan li</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>追加图片</t>
+    <rPh sb="2" eb="3">
+      <t>tu p</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除图片</t>
+    <rPh sb="2" eb="3">
+      <t>tu p</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品管理 - 图片管理</t>
+    <rPh sb="7" eb="8">
+      <t>tu p</t>
+    </rPh>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -417,6 +456,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="25">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -429,19 +469,18 @@
     <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -740,13 +779,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="29.5" style="1" bestFit="1" customWidth="1"/>
@@ -755,12 +794,12 @@
     <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -771,7 +810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>11000</v>
       </c>
@@ -782,7 +821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>11001</v>
       </c>
@@ -793,7 +832,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>11002</v>
       </c>
@@ -804,7 +843,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>11003</v>
       </c>
@@ -815,7 +854,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>12000</v>
       </c>
@@ -826,7 +865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>12100</v>
       </c>
@@ -837,7 +876,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>12200</v>
       </c>
@@ -848,7 +887,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>12300</v>
       </c>
@@ -859,7 +898,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>12301</v>
       </c>
@@ -870,7 +909,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>12302</v>
       </c>
@@ -881,7 +920,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>12303</v>
       </c>
@@ -898,7 +937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>12400</v>
       </c>
@@ -909,7 +948,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>13000</v>
       </c>
@@ -920,7 +959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>13100</v>
       </c>
@@ -931,7 +970,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>13101</v>
       </c>
@@ -942,7 +981,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>13102</v>
       </c>
@@ -953,7 +992,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>13103</v>
       </c>
@@ -964,7 +1003,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>13104</v>
       </c>
@@ -975,7 +1014,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>13200</v>
       </c>
@@ -986,7 +1025,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>13201</v>
       </c>
@@ -997,7 +1036,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>13202</v>
       </c>
@@ -1008,7 +1047,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>13203</v>
       </c>
@@ -1019,7 +1058,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>13204</v>
       </c>
@@ -1030,7 +1069,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>13205</v>
       </c>
@@ -1047,7 +1086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <v>13300</v>
       </c>
@@ -1058,7 +1097,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>13302</v>
       </c>
@@ -1069,7 +1108,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <v>13303</v>
       </c>
@@ -1080,7 +1119,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <v>13304</v>
       </c>
@@ -1091,7 +1130,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <v>13400</v>
       </c>
@@ -1108,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
         <v>13402</v>
       </c>
@@ -1125,7 +1164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
         <v>13404</v>
       </c>
@@ -1142,47 +1181,80 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
+        <v>13500</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A36" s="3">
+        <v>13502</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A37" s="3">
+        <v>13503</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A38" s="3">
         <v>14000</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A39" s="3">
         <v>15000</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A40" s="3">
         <v>15100</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A41" s="3">
         <v>15200</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1190,10 +1262,5 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>